<commit_message>
error at date values
</commit_message>
<xml_diff>
--- a/model2/07.2022---05.2024.xlsx
+++ b/model2/07.2022---05.2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismat\Рабочий стол\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismat\Budget_Analyse\model2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22351052-0059-4EA0-8E49-1E75042E9FBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DE4203-A41E-4A4D-8BB8-258A58759067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,15 +391,15 @@
   <dimension ref="A1:D2780"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>